<commit_message>
Design e pagina de web scraping com atualizações
</commit_message>
<xml_diff>
--- a/backEnd/webScraping/Backup/instiglio.xlsx
+++ b/backEnd/webScraping/Backup/instiglio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,19 +590,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.instiglio.org/en/ve-dib/</t>
+          <t>https://www.instiglio.org/en/foster-care-in-chile/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
-        <is>
-          <t>https://www.instiglio.org/en/foster-care-in-chile/</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
         <is>
           <t>https://www.instiglio.org/en/entrepreneurship-in-medellin-colombia/</t>
         </is>

</xml_diff>